<commit_message>
feat: Complete Phase 3 test execution with comprehensive bug documentation
- Add TEST_EXECUTION_GUIDELINES.md with structured testing framework
- Create 10 detailed bug reports (BUG001-BUG010) documenting critical defects
- Consolidate all findings in DefectReports.md
- Include evidence images and descriptions for all identified issues
- Document security vulnerabilities, session management issues, and data integrity problems
- Establish bug tracking system and documentation structure
</commit_message>
<xml_diff>
--- a/docs/source-documents/TestCaseExecution_Summary.xlsx
+++ b/docs/source-documents/TestCaseExecution_Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotch3/Documents/MENTORIAQA2.0/projetos/portfolio-project/bookingmate/docs/source-documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4055C8-B659-2B4D-AA85-1009A3D40F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998588D5-B70C-2F49-9849-51D18CF226A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3560" windowWidth="38400" windowHeight="21100" xr2:uid="{484DA1DC-CF6B-E941-8264-03655C04B066}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="26880" windowHeight="16320" xr2:uid="{484DA1DC-CF6B-E941-8264-03655C04B066}"/>
   </bookViews>
   <sheets>
     <sheet name="Test case execution summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
   <si>
     <t>TC ID</t>
   </si>
@@ -220,6 +220,21 @@
   </si>
   <si>
     <t>BUG002</t>
+  </si>
+  <si>
+    <t>Reservation's day displayed in reservations list is incorrect</t>
+  </si>
+  <si>
+    <t>BUG003</t>
+  </si>
+  <si>
+    <t>BUG004</t>
+  </si>
+  <si>
+    <t>BUG008</t>
+  </si>
+  <si>
+    <t>BUG007</t>
   </si>
 </sst>
 </file>
@@ -343,15 +358,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E89E1BFC-249F-4142-97B2-E91FA14D2740}" name="Tabela2" displayName="Tabela2" ref="C3:H24" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E89E1BFC-249F-4142-97B2-E91FA14D2740}" name="Tabela2" displayName="Tabela2" ref="C3:H24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="C3:H24" xr:uid="{E89E1BFC-249F-4142-97B2-E91FA14D2740}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A61A7AEF-5D42-7E49-A102-FC82050CEEC1}" name="TC ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8E14B110-4EBB-B542-B300-46233C2C0BDC}" name="Priority" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{278FCE19-6F73-E245-8513-6E7A5137DEDA}" name="Title" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{E2534804-4011-D149-815D-6EF00CA161E8}" name="Status" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{6F652E42-3FDF-FE45-B607-5261DC42B8AF}" name="Defect ID" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{0631E536-AF42-D344-AC05-CB6B4F368B26}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A61A7AEF-5D42-7E49-A102-FC82050CEEC1}" name="TC ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8E14B110-4EBB-B542-B300-46233C2C0BDC}" name="Priority" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{278FCE19-6F73-E245-8513-6E7A5137DEDA}" name="Title" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E2534804-4011-D149-815D-6EF00CA161E8}" name="Status" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{6F652E42-3FDF-FE45-B607-5261DC42B8AF}" name="Defect ID" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{0631E536-AF42-D344-AC05-CB6B4F368B26}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -676,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DAD545-DA48-DA44-B081-A12C97D48F8A}">
   <dimension ref="B3:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,7 +727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -723,11 +738,15 @@
       <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="F4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
@@ -780,7 +799,7 @@
         <v>50</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>58</v>
@@ -797,10 +816,12 @@
       <c r="E8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="3"/>
+      <c r="F8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="2:8" ht="34" x14ac:dyDescent="0.2">
@@ -869,7 +890,7 @@
         <v>53</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>54</v>
@@ -889,7 +910,9 @@
       <c r="F13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="H13" s="3" t="s">
         <v>55</v>
       </c>
@@ -908,7 +931,9 @@
       <c r="F14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="H14" s="3" t="s">
         <v>56</v>
       </c>
@@ -944,7 +969,9 @@
       <c r="F16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="2:8" ht="17" x14ac:dyDescent="0.2">
@@ -961,7 +988,9 @@
       <c r="F17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="2:8" ht="17" x14ac:dyDescent="0.2">
@@ -1012,7 +1041,9 @@
       <c r="F20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="3"/>
+      <c r="G20" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="2:8" ht="34" x14ac:dyDescent="0.2">

</xml_diff>